<commit_message>
Merge branches 'RDM-2053' and 'master' of github.com:hmcts/ccd-definition-store-api into RDM-2053
# Conflicts:
#	application/src/test/resources/CCD_TestDefinition_V26_RDM-1473.xlsx
#	repository/src/main/resources/db/changelog/db.changelog-master.xml
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V30.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V30.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="29005"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrzejfolga/src/ccd/temp/ccd-definition-store-api/application/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fatiho/Documents/hmcts/workspace/ccd-definition-store-api/application/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2261D5-982A-7341-A73D-AE183B77C956}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5640" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="-5080" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -31,7 +32,7 @@
     <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId17"/>
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="277">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -879,11 +880,23 @@
   <si>
     <t>Boolean expression rules for hiding a tab: MaxLength:1000</t>
   </si>
+  <si>
+    <t>EndButtonLabel</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Create Draft</t>
+  </si>
+  <si>
+    <t>Text value to show while submitting the event form data</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
     <numFmt numFmtId="165" formatCode="d\/m\/yy"/>
@@ -1364,7 +1377,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1543,6 +1556,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1925,7 +1942,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -2151,7 +2168,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -2513,7 +2530,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2827,7 +2844,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -3190,7 +3207,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
@@ -3899,7 +3916,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
@@ -4097,8 +4114,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C5" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4109,7 +4126,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:IU10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -6776,7 +6793,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -7742,7 +7759,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:IU15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -11770,7 +11787,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:IU15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -12654,7 +12671,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -13022,7 +13039,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
@@ -14306,7 +14323,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
@@ -14651,7 +14668,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -15575,7 +15592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -15955,10 +15972,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -15966,12 +15985,12 @@
     <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="45.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="45.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="29.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="27.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="32" style="1" customWidth="1"/>
     <col min="12" max="12" width="31.5" style="1" customWidth="1"/>
     <col min="13" max="13" width="29.83203125" style="1" customWidth="1"/>
@@ -15979,7 +15998,8 @@
     <col min="15" max="15" width="29.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="23.6640625" style="1" customWidth="1"/>
     <col min="17" max="17" width="31.1640625" style="1" customWidth="1"/>
-    <col min="18" max="21" width="8.83203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.33203125" style="1" customWidth="1"/>
+    <col min="19" max="21" width="8.83203125" style="1" customWidth="1"/>
     <col min="22" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16009,12 +16029,12 @@
       <c r="O1" s="41"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
+      <c r="R1" s="120"/>
       <c r="S1" s="4"/>
       <c r="T1" s="4"/>
       <c r="U1" s="4"/>
     </row>
-    <row r="2" spans="1:21" ht="65" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" ht="155" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -16062,7 +16082,9 @@
       <c r="Q2" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="R2" s="5"/>
+      <c r="R2" s="127" t="s">
+        <v>276</v>
+      </c>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
@@ -16119,7 +16141,9 @@
       <c r="Q3" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="R3" s="8"/>
+      <c r="R3" s="126" t="s">
+        <v>273</v>
+      </c>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
       <c r="U3" s="8"/>
@@ -16160,7 +16184,9 @@
       <c r="Q4" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="R4" s="4"/>
+      <c r="R4" s="120" t="s">
+        <v>274</v>
+      </c>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
@@ -16203,7 +16229,9 @@
       <c r="Q5" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="R5" s="4"/>
+      <c r="R5" s="120" t="s">
+        <v>275</v>
+      </c>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
@@ -16246,7 +16274,7 @@
       <c r="Q6" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="R6" s="4"/>
+      <c r="R6" s="120"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
@@ -16287,7 +16315,7 @@
       <c r="Q7" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="R7" s="4"/>
+      <c r="R7" s="120"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
@@ -16330,7 +16358,7 @@
       <c r="Q8" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="R8" s="4"/>
+      <c r="R8" s="120"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
@@ -16371,7 +16399,7 @@
         <v>49</v>
       </c>
       <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
+      <c r="R9" s="120"/>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
@@ -16394,7 +16422,7 @@
       <c r="O10" s="41"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
+      <c r="R10" s="120"/>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
@@ -16417,7 +16445,7 @@
       <c r="O11" s="41"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
+      <c r="R11" s="120"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
@@ -16440,7 +16468,7 @@
       <c r="O12" s="41"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
+      <c r="R12" s="120"/>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
@@ -16463,7 +16491,7 @@
       <c r="O13" s="41"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
+      <c r="R13" s="120"/>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
@@ -16486,7 +16514,7 @@
       <c r="O14" s="41"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
+      <c r="R14" s="120"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
@@ -16509,7 +16537,7 @@
       <c r="O15" s="41"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
+      <c r="R15" s="120"/>
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
@@ -16532,7 +16560,7 @@
       <c r="O16" s="41"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
+      <c r="R16" s="120"/>
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
@@ -16555,7 +16583,7 @@
       <c r="O17" s="41"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
+      <c r="R17" s="120"/>
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
@@ -16578,7 +16606,7 @@
       <c r="O18" s="41"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
+      <c r="R18" s="120"/>
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
@@ -16601,7 +16629,7 @@
       <c r="O19" s="41"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
+      <c r="R19" s="120"/>
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
@@ -16616,10 +16644,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="119" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
@@ -16632,10 +16660,11 @@
     <col min="5" max="5" width="19.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" style="1" customWidth="1"/>
     <col min="7" max="8" width="17.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="29.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" style="1" customWidth="1"/>
     <col min="10" max="11" width="20.1640625" style="1" customWidth="1"/>
-    <col min="12" max="13" width="22" style="1" customWidth="1"/>
-    <col min="14" max="14" width="45.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="22" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.1640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5" style="1" customWidth="1"/>
     <col min="15" max="17" width="8.83203125" style="1" customWidth="1"/>
     <col min="18" max="1024" width="8.83203125" customWidth="1"/>
   </cols>
@@ -17205,7 +17234,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">

</xml_diff>